<commit_message>
Tambah Role Upload Excel User
</commit_message>
<xml_diff>
--- a/public/assets/import/format/user.xlsx
+++ b/public/assets/import/format/user.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46aa635a8be11eab/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6E53F4-ADAA-4F76-BF9E-C494607BB7D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{DC6E53F4-ADAA-4F76-BF9E-C494607BB7D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CDEC4D9F-5D83-439B-9787-F44FA21F6142}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5DBE6DA8-71C1-49DD-AF16-D5C89A017676}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nama</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>no_induk</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pengampu</t>
+  </si>
+  <si>
+    <t>peserta</t>
   </si>
 </sst>
 </file>
@@ -78,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,19 +404,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AFE67C-BAD9-45C7-B3FF-A10640795D11}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -425,9 +437,21 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{E7E11919-E636-46C2-BAAB-733FF8D8D1C5}">
       <formula1>"Laki-laki, Perempuan"</formula1>
     </dataValidation>
@@ -437,6 +461,9 @@
     <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{B845C6DA-1E4F-4FF6-AB10-BE1769975548}">
       <formula1>12</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:I1048576" xr:uid="{1258E96B-7635-438F-A1AA-2491E80A4A08}">
+      <formula1>"Ya, Tidak,"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>